<commit_message>
Update time tracking sheet with latest contributions as well as backend requirements document with notes and to do list for categories
</commit_message>
<xml_diff>
--- a/CP317 Time Tracking Sheet.xlsx
+++ b/CP317 Time Tracking Sheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26408"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roman/Documents/romanlipisiy/github/virtual-environment/UPOD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/WillDetlor/GitHub/UPOD/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="337">
   <si>
     <t>Raw</t>
   </si>
@@ -1230,6 +1230,9 @@
   </si>
   <si>
     <t>07/01/16 - Migrated vapourware files to ruby on rails scaffolding</t>
+  </si>
+  <si>
+    <t>Organizing categories/sub-categories design, developing requirements document with results of discussions</t>
   </si>
 </sst>
 </file>
@@ -1352,11 +1355,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1689,8 +1692,8 @@
   <dimension ref="A1:I1005"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H151" sqref="H151"/>
+      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D153" sqref="D153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1775,10 +1778,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve"> 17:38</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="23"/>
+      <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:9" ht="39" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
@@ -1804,8 +1807,8 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve"> 18:03</v>
       </c>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
@@ -4964,16 +4967,30 @@
         <v>335</v>
       </c>
       <c r="E151" s="14"/>
-      <c r="F151" s="24">
+      <c r="F151" s="22">
         <v>42552</v>
       </c>
       <c r="G151" s="17">
         <v>0.15625</v>
       </c>
     </row>
-    <row r="152" spans="2:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="152" spans="2:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="B152" t="s">
+        <v>64</v>
+      </c>
+      <c r="C152" s="1">
+        <v>3</v>
+      </c>
+      <c r="D152" s="21" t="s">
+        <v>336</v>
+      </c>
       <c r="E152" s="14"/>
-      <c r="G152" s="17"/>
+      <c r="F152" s="22">
+        <v>42555</v>
+      </c>
+      <c r="G152" s="17">
+        <v>0.74305555555555547</v>
+      </c>
     </row>
     <row r="153" spans="2:7" ht="13" x14ac:dyDescent="0.15">
       <c r="E153" s="14"/>

</xml_diff>